<commit_message>
Add admin options for Excel file upload and status reset
- Add new admin section in super admin panel
- Excel file upload with backup and validation
- Status reset with multiple confirmations
- Backend endpoints for both features
</commit_message>
<xml_diff>
--- a/data/registrations.xlsx
+++ b/data/registrations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="433">
   <si>
     <t>Registration No</t>
   </si>
@@ -1015,19 +1015,22 @@
     <t>Syed Idrees</t>
   </si>
   <si>
+    <t>gowtham</t>
+  </si>
+  <si>
+    <t>Barsa</t>
+  </si>
+  <si>
+    <t>Bhavishya Gowda</t>
+  </si>
+  <si>
+    <t>Dhruv Singh</t>
+  </si>
+  <si>
+    <t>Jahnavi</t>
+  </si>
+  <si>
     <t>Ananya</t>
-  </si>
-  <si>
-    <t>Barsa</t>
-  </si>
-  <si>
-    <t>Bhavishya Gowda</t>
-  </si>
-  <si>
-    <t>Dhruv Singh</t>
-  </si>
-  <si>
-    <t>Jahnavi</t>
   </si>
   <si>
     <t>Shalin</t>
@@ -1877,10 +1880,10 @@
         <v>46046.36974537037</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AF2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="AG2">
         <v>250</v>
@@ -1889,19 +1892,19 @@
         <v>46043.59777777778</v>
       </c>
       <c r="AI2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AK2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="AL2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AM2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:45">
@@ -1954,7 +1957,7 @@
         <v>46046.36947916666</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG3">
         <v>250</v>
@@ -1963,19 +1966,19 @@
         <v>46046.59512731482</v>
       </c>
       <c r="AI3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AL3" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AM3" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AN3" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:45">
@@ -2019,7 +2022,7 @@
         <v>333</v>
       </c>
       <c r="P4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="Z4">
         <v>500</v>
@@ -2037,25 +2040,25 @@
         <v>46047.57050925926</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG4">
         <v>500</v>
       </c>
       <c r="AI4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AL4" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AM4" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -2108,25 +2111,25 @@
         <v>46048.17354166666</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG5">
         <v>250</v>
       </c>
       <c r="AI5" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AL5" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AM5" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AN5" s="3" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="6" spans="1:45">
@@ -2176,25 +2179,25 @@
         <v>46048.70457175926</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG6">
         <v>2000</v>
       </c>
       <c r="AI6" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK6" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AL6" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AM6" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AN6" s="3" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -2247,25 +2250,25 @@
         <v>46048.73724537037</v>
       </c>
       <c r="AE7" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG7">
         <v>1500</v>
       </c>
       <c r="AI7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK7" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AL7" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM7" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AN7" s="3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="8" spans="1:45">
@@ -2318,25 +2321,25 @@
         <v>46050.5496412037</v>
       </c>
       <c r="AE8" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG8">
         <v>500</v>
       </c>
       <c r="AI8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK8" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AL8" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AM8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AN8" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:45">
@@ -2380,7 +2383,7 @@
         <v>334</v>
       </c>
       <c r="P9" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="Z9">
         <v>500</v>
@@ -2395,25 +2398,25 @@
         <v>46050.5603125</v>
       </c>
       <c r="AE9" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG9">
         <v>500</v>
       </c>
       <c r="AI9" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK9" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AL9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AM9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AN9" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="10" spans="1:45">
@@ -2469,25 +2472,25 @@
         <v>46051.26159722222</v>
       </c>
       <c r="AE10" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG10">
         <v>500</v>
       </c>
       <c r="AI10" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK10" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AL10" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AM10" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AN10" s="3" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:45">
@@ -2546,25 +2549,25 @@
         <v>46052.85017361111</v>
       </c>
       <c r="AE11" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG11">
         <v>500</v>
       </c>
       <c r="AI11" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK11" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AL11" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AM11" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AN11" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="12" spans="1:45">
@@ -2614,25 +2617,25 @@
         <v>46053.32211805556</v>
       </c>
       <c r="AE12" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG12">
         <v>1500</v>
       </c>
       <c r="AI12" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK12" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AL12" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AM12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AN12" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="1:45">
@@ -2688,25 +2691,25 @@
         <v>46053.68641203704</v>
       </c>
       <c r="AE13" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG13">
         <v>250</v>
       </c>
       <c r="AI13" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK13" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AL13" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AM13" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AN13" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14" spans="1:45">
@@ -2759,25 +2762,25 @@
         <v>46054.20597222223</v>
       </c>
       <c r="AE14" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG14">
         <v>250</v>
       </c>
       <c r="AI14" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK14" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AL14" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AM14" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AN14" s="3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="15" spans="1:45">
@@ -2830,25 +2833,25 @@
         <v>46054.20864583334</v>
       </c>
       <c r="AE15" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG15">
         <v>250</v>
       </c>
       <c r="AI15" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK15" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AL15" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AM15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AN15" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="16" spans="1:45">
@@ -2901,10 +2904,10 @@
         <v>46055.22414351852</v>
       </c>
       <c r="AE16" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AF16" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="AG16">
         <v>250</v>
@@ -2913,19 +2916,19 @@
         <v>46055.45304398148</v>
       </c>
       <c r="AI16" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AK16" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AL16" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AM16" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AN16" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="17" spans="1:40">
@@ -2978,10 +2981,10 @@
         <v>46055.33483796296</v>
       </c>
       <c r="AE17" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AF17" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AG17">
         <v>250</v>
@@ -2990,19 +2993,19 @@
         <v>46055.56552083333</v>
       </c>
       <c r="AI17" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AK17" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AL17" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AM17" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AN17" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="18" spans="1:40">
@@ -3055,10 +3058,10 @@
         <v>46055.335625</v>
       </c>
       <c r="AE18" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AF18" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AG18">
         <v>250</v>
@@ -3067,19 +3070,19 @@
         <v>46055.56576388889</v>
       </c>
       <c r="AI18" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AK18" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AL18" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AM18" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AN18" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="19" spans="1:40">
@@ -3123,10 +3126,10 @@
         <v>335</v>
       </c>
       <c r="P19" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q19" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="Z19">
         <v>500</v>
@@ -3141,10 +3144,10 @@
         <v>46055.34297453704</v>
       </c>
       <c r="AE19" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AF19" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AG19">
         <v>500</v>
@@ -3153,19 +3156,19 @@
         <v>46055.57255787037</v>
       </c>
       <c r="AI19" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AK19" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AL19" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AM19" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AN19" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="20" spans="1:40">
@@ -3209,10 +3212,10 @@
         <v>336</v>
       </c>
       <c r="P20" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q20" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="Z20">
         <v>500</v>
@@ -3227,10 +3230,10 @@
         <v>46055.34579861111</v>
       </c>
       <c r="AE20" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AF20" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AG20">
         <v>500</v>
@@ -3239,19 +3242,19 @@
         <v>46055.57982638889</v>
       </c>
       <c r="AI20" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AK20" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AL20" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AM20" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AN20" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="21" spans="1:40">
@@ -3304,22 +3307,22 @@
         <v>46056.26671296296</v>
       </c>
       <c r="AE21" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG21">
         <v>250</v>
       </c>
       <c r="AK21" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AL21" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AM21" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AN21" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="22" spans="1:40">
@@ -3372,10 +3375,10 @@
         <v>46056.27141203704</v>
       </c>
       <c r="AE22" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AF22" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AG22">
         <v>250</v>
@@ -3384,19 +3387,19 @@
         <v>46056.50103009259</v>
       </c>
       <c r="AI22" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AK22" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AL22" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AM22" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AN22" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="23" spans="1:40">
@@ -3452,22 +3455,22 @@
         <v>46056.2725</v>
       </c>
       <c r="AE23" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG23">
         <v>250</v>
       </c>
       <c r="AK23" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AL23" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AM23" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AN23" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="24" spans="1:40">
@@ -3511,7 +3514,7 @@
         <v>337</v>
       </c>
       <c r="P24" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="Z24">
         <v>500</v>
@@ -3526,22 +3529,22 @@
         <v>46056.33609953704</v>
       </c>
       <c r="AE24" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG24">
         <v>500</v>
       </c>
       <c r="AK24" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AL24" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AM24" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AN24" s="3" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="25" spans="1:40">
@@ -3658,10 +3661,10 @@
         <v>319</v>
       </c>
       <c r="O27" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="P27" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:40">
@@ -3854,7 +3857,7 @@
         <v>334</v>
       </c>
       <c r="P32" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -4249,10 +4252,10 @@
         <v>335</v>
       </c>
       <c r="P42" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q42" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -4296,10 +4299,10 @@
         <v>336</v>
       </c>
       <c r="P43" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q43" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -4460,7 +4463,7 @@
         <v>337</v>
       </c>
       <c r="P47" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -4577,10 +4580,10 @@
         <v>319</v>
       </c>
       <c r="O50" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="P50" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -4773,7 +4776,7 @@
         <v>334</v>
       </c>
       <c r="P55" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -5168,10 +5171,10 @@
         <v>335</v>
       </c>
       <c r="P65" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q65" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="66" spans="1:17">
@@ -5215,10 +5218,10 @@
         <v>336</v>
       </c>
       <c r="P66" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q66" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="67" spans="1:17">
@@ -5379,7 +5382,7 @@
         <v>337</v>
       </c>
       <c r="P70" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="71" spans="1:17">
@@ -5496,10 +5499,10 @@
         <v>319</v>
       </c>
       <c r="O73" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="P73" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="74" spans="1:17">
@@ -5692,7 +5695,7 @@
         <v>334</v>
       </c>
       <c r="P78" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="79" spans="1:17">
@@ -6087,10 +6090,10 @@
         <v>335</v>
       </c>
       <c r="P88" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q88" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="89" spans="1:17">
@@ -6134,10 +6137,10 @@
         <v>336</v>
       </c>
       <c r="P89" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q89" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="90" spans="1:17">
@@ -6298,7 +6301,7 @@
         <v>337</v>
       </c>
       <c r="P93" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="94" spans="1:17">
@@ -6415,10 +6418,10 @@
         <v>319</v>
       </c>
       <c r="O96" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="P96" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="97" spans="1:17">
@@ -6611,7 +6614,7 @@
         <v>334</v>
       </c>
       <c r="P101" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="102" spans="1:17">
@@ -7006,10 +7009,10 @@
         <v>335</v>
       </c>
       <c r="P111" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q111" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="112" spans="1:17">
@@ -7053,10 +7056,10 @@
         <v>336</v>
       </c>
       <c r="P112" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q112" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="113" spans="1:16">
@@ -7217,7 +7220,7 @@
         <v>337</v>
       </c>
       <c r="P116" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="117" spans="1:16">
@@ -7334,10 +7337,10 @@
         <v>319</v>
       </c>
       <c r="O119" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="P119" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="120" spans="1:16">
@@ -7530,7 +7533,7 @@
         <v>334</v>
       </c>
       <c r="P124" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="125" spans="1:16">
@@ -7925,10 +7928,10 @@
         <v>335</v>
       </c>
       <c r="P134" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q134" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="135" spans="1:17">
@@ -7972,10 +7975,10 @@
         <v>336</v>
       </c>
       <c r="P135" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q135" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="136" spans="1:17">
@@ -8136,7 +8139,7 @@
         <v>337</v>
       </c>
       <c r="P139" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="140" spans="1:17">
@@ -8253,10 +8256,10 @@
         <v>319</v>
       </c>
       <c r="O142" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="P142" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="143" spans="1:17">
@@ -8449,7 +8452,7 @@
         <v>334</v>
       </c>
       <c r="P147" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="148" spans="1:17">
@@ -8844,10 +8847,10 @@
         <v>335</v>
       </c>
       <c r="P157" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q157" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="158" spans="1:17">
@@ -8891,10 +8894,10 @@
         <v>336</v>
       </c>
       <c r="P158" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q158" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="159" spans="1:17">
@@ -9055,7 +9058,7 @@
         <v>337</v>
       </c>
       <c r="P162" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="163" spans="1:16">
@@ -9172,10 +9175,10 @@
         <v>319</v>
       </c>
       <c r="O165" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="P165" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="166" spans="1:16">
@@ -9368,7 +9371,7 @@
         <v>334</v>
       </c>
       <c r="P170" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="171" spans="1:16">
@@ -9763,10 +9766,10 @@
         <v>335</v>
       </c>
       <c r="P180" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q180" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="181" spans="1:17">
@@ -9810,10 +9813,10 @@
         <v>336</v>
       </c>
       <c r="P181" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q181" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="182" spans="1:17">
@@ -9974,7 +9977,7 @@
         <v>337</v>
       </c>
       <c r="P185" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="186" spans="1:17">
@@ -10091,10 +10094,10 @@
         <v>319</v>
       </c>
       <c r="O188" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="P188" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="189" spans="1:17">
@@ -10287,7 +10290,7 @@
         <v>334</v>
       </c>
       <c r="P193" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="194" spans="1:16">

</xml_diff>